<commit_message>
Iniciando a geração de gráficos e tabelas para o artigo e apresentação
</commit_message>
<xml_diff>
--- a/Testes/PingPing/PingPing.xlsx
+++ b/Testes/PingPing/PingPing.xlsx
@@ -783,11 +783,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68582016"/>
-        <c:axId val="68596096"/>
+        <c:axId val="63416960"/>
+        <c:axId val="63435520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68582016"/>
+        <c:axId val="63416960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -816,7 +816,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68596096"/>
+        <c:crossAx val="63435520"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -824,7 +824,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68596096"/>
+        <c:axId val="63435520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +854,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68582016"/>
+        <c:crossAx val="63416960"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1077,11 +1077,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="208513664"/>
-        <c:axId val="208667392"/>
+        <c:axId val="64181760"/>
+        <c:axId val="64183680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208513664"/>
+        <c:axId val="64181760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,7 +1110,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208667392"/>
+        <c:crossAx val="64183680"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1118,7 +1118,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208667392"/>
+        <c:axId val="64183680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1148,7 +1148,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208513664"/>
+        <c:crossAx val="64181760"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1675,11 +1675,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209038720"/>
-        <c:axId val="209212160"/>
+        <c:axId val="64253952"/>
+        <c:axId val="64255872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209038720"/>
+        <c:axId val="64253952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1708,7 +1708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209212160"/>
+        <c:crossAx val="64255872"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1716,7 +1716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209212160"/>
+        <c:axId val="64255872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1746,7 +1746,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209038720"/>
+        <c:crossAx val="64253952"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2121,11 +2121,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209203968"/>
-        <c:axId val="162541952"/>
+        <c:axId val="63509632"/>
+        <c:axId val="63511552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209203968"/>
+        <c:axId val="63509632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2154,7 +2154,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162541952"/>
+        <c:crossAx val="63511552"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2162,7 +2162,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162541952"/>
+        <c:axId val="63511552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2192,7 +2192,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209203968"/>
+        <c:crossAx val="63509632"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2415,11 +2415,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="209086336"/>
-        <c:axId val="209115008"/>
+        <c:axId val="63541632"/>
+        <c:axId val="63543552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="209086336"/>
+        <c:axId val="63541632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2448,7 +2448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209115008"/>
+        <c:crossAx val="63543552"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2456,7 +2456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209115008"/>
+        <c:axId val="63543552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2486,7 +2486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209086336"/>
+        <c:crossAx val="63541632"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3013,11 +3013,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="206886016"/>
-        <c:axId val="206938496"/>
+        <c:axId val="63662720"/>
+        <c:axId val="63681280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="206886016"/>
+        <c:axId val="63662720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3046,7 +3046,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206938496"/>
+        <c:crossAx val="63681280"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3054,7 +3054,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206938496"/>
+        <c:axId val="63681280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3084,7 +3084,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206886016"/>
+        <c:crossAx val="63662720"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3459,11 +3459,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="165672448"/>
-        <c:axId val="165674368"/>
+        <c:axId val="63590400"/>
+        <c:axId val="63592320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="165672448"/>
+        <c:axId val="63590400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3492,7 +3492,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165674368"/>
+        <c:crossAx val="63592320"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3500,7 +3500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165674368"/>
+        <c:axId val="63592320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3530,7 +3530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165672448"/>
+        <c:crossAx val="63590400"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3753,11 +3753,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97222016"/>
-        <c:axId val="97883648"/>
+        <c:axId val="63618048"/>
+        <c:axId val="63620224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97222016"/>
+        <c:axId val="63618048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3786,7 +3786,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97883648"/>
+        <c:crossAx val="63620224"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3794,7 +3794,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97883648"/>
+        <c:axId val="63620224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3824,7 +3824,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97222016"/>
+        <c:crossAx val="63618048"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4427,11 +4427,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68779392"/>
-        <c:axId val="68785280"/>
+        <c:axId val="63219584"/>
+        <c:axId val="63221760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68779392"/>
+        <c:axId val="63219584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4460,7 +4460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68785280"/>
+        <c:crossAx val="63221760"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4468,7 +4468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68785280"/>
+        <c:axId val="63221760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4498,7 +4498,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68779392"/>
+        <c:crossAx val="63219584"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5101,11 +5101,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69292032"/>
-        <c:axId val="69293568"/>
+        <c:axId val="63743104"/>
+        <c:axId val="63745024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69292032"/>
+        <c:axId val="63743104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5134,7 +5134,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69293568"/>
+        <c:crossAx val="63745024"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5142,7 +5142,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69293568"/>
+        <c:axId val="63745024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5172,7 +5172,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69292032"/>
+        <c:crossAx val="63743104"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5787,11 +5787,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69540480"/>
-        <c:axId val="69542272"/>
+        <c:axId val="63909888"/>
+        <c:axId val="63912192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69540480"/>
+        <c:axId val="63909888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5820,7 +5820,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69542272"/>
+        <c:crossAx val="63912192"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5828,7 +5828,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69542272"/>
+        <c:axId val="63912192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5858,7 +5858,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69540480"/>
+        <c:crossAx val="63909888"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6390,11 +6390,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69583232"/>
-        <c:axId val="69584768"/>
+        <c:axId val="63957632"/>
+        <c:axId val="63836928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69583232"/>
+        <c:axId val="63957632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6423,7 +6423,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69584768"/>
+        <c:crossAx val="63836928"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6431,7 +6431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69584768"/>
+        <c:axId val="63836928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6461,7 +6461,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69583232"/>
+        <c:crossAx val="63957632"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6836,11 +6836,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="208159104"/>
-        <c:axId val="208161408"/>
+        <c:axId val="63881216"/>
+        <c:axId val="63883136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208159104"/>
+        <c:axId val="63881216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6869,7 +6869,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208161408"/>
+        <c:crossAx val="63883136"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6877,7 +6877,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="208161408"/>
+        <c:axId val="63883136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6907,7 +6907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208159104"/>
+        <c:crossAx val="63881216"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7130,11 +7130,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="97382784"/>
-        <c:axId val="97384704"/>
+        <c:axId val="63986688"/>
+        <c:axId val="63992960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97382784"/>
+        <c:axId val="63986688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7163,7 +7163,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97384704"/>
+        <c:crossAx val="63992960"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7171,7 +7171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97384704"/>
+        <c:axId val="63992960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7201,7 +7201,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97382784"/>
+        <c:crossAx val="63986688"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7728,11 +7728,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="94372992"/>
-        <c:axId val="97310592"/>
+        <c:axId val="64108032"/>
+        <c:axId val="64109952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94372992"/>
+        <c:axId val="64108032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7761,7 +7761,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97310592"/>
+        <c:crossAx val="64109952"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7769,7 +7769,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97310592"/>
+        <c:axId val="64109952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7799,7 +7799,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94372992"/>
+        <c:crossAx val="64108032"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8174,11 +8174,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="208999552"/>
-        <c:axId val="209084800"/>
+        <c:axId val="64145664"/>
+        <c:axId val="64156032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208999552"/>
+        <c:axId val="64145664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8207,7 +8207,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209084800"/>
+        <c:crossAx val="64156032"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8215,7 +8215,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="209084800"/>
+        <c:axId val="64156032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8245,7 +8245,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208999552"/>
+        <c:crossAx val="64145664"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9063,7 +9063,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CI232"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="BR54" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="CK110" sqref="CK110"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Atualizado documento com gráficos e tabelas de PingPing e PingPong
</commit_message>
<xml_diff>
--- a/Testes/PingPing/PingPing.xlsx
+++ b/Testes/PingPing/PingPing.xlsx
@@ -209,10 +209,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -783,11 +783,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63416960"/>
-        <c:axId val="63435520"/>
+        <c:axId val="203879936"/>
+        <c:axId val="203881856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63416960"/>
+        <c:axId val="203879936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -816,7 +816,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63435520"/>
+        <c:crossAx val="203881856"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -824,7 +824,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63435520"/>
+        <c:axId val="203881856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +854,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63416960"/>
+        <c:crossAx val="203879936"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -870,7 +870,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -883,10 +883,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1077,11 +1077,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="64181760"/>
-        <c:axId val="64183680"/>
+        <c:axId val="204331264"/>
+        <c:axId val="204345728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64181760"/>
+        <c:axId val="204331264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1110,7 +1110,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64183680"/>
+        <c:crossAx val="204345728"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1118,7 +1118,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64183680"/>
+        <c:axId val="204345728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1148,7 +1148,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64181760"/>
+        <c:crossAx val="204331264"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1164,7 +1164,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1177,10 +1177,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1675,11 +1675,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="64253952"/>
-        <c:axId val="64255872"/>
+        <c:axId val="204413952"/>
+        <c:axId val="204428416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64253952"/>
+        <c:axId val="204413952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1708,7 +1708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64255872"/>
+        <c:crossAx val="204428416"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1716,7 +1716,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64255872"/>
+        <c:axId val="204428416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1746,7 +1746,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64253952"/>
+        <c:crossAx val="204413952"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1762,7 +1762,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1775,10 +1775,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -2121,11 +2121,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63509632"/>
-        <c:axId val="63511552"/>
+        <c:axId val="204470144"/>
+        <c:axId val="205008896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63509632"/>
+        <c:axId val="204470144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2154,7 +2154,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63511552"/>
+        <c:crossAx val="205008896"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2162,7 +2162,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63511552"/>
+        <c:axId val="205008896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2192,7 +2192,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63509632"/>
+        <c:crossAx val="204470144"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2208,7 +2208,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2221,10 +2221,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -2415,11 +2415,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63541632"/>
-        <c:axId val="63543552"/>
+        <c:axId val="205039488"/>
+        <c:axId val="205041664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63541632"/>
+        <c:axId val="205039488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2448,7 +2448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63543552"/>
+        <c:crossAx val="205041664"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2456,7 +2456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63543552"/>
+        <c:axId val="205041664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2486,7 +2486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63541632"/>
+        <c:crossAx val="205039488"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2502,7 +2502,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2515,10 +2515,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -3013,11 +3013,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63662720"/>
-        <c:axId val="63681280"/>
+        <c:axId val="205171328"/>
+        <c:axId val="205071104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63662720"/>
+        <c:axId val="205171328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3046,7 +3046,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63681280"/>
+        <c:crossAx val="205071104"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3054,7 +3054,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63681280"/>
+        <c:axId val="205071104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3084,7 +3084,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63662720"/>
+        <c:crossAx val="205171328"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3100,7 +3100,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3113,10 +3113,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -3459,11 +3459,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63590400"/>
-        <c:axId val="63592320"/>
+        <c:axId val="205104640"/>
+        <c:axId val="205106560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63590400"/>
+        <c:axId val="205104640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3492,7 +3492,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63592320"/>
+        <c:crossAx val="205106560"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3500,7 +3500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63592320"/>
+        <c:axId val="205106560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3530,7 +3530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63590400"/>
+        <c:crossAx val="205104640"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3546,7 +3546,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3559,10 +3559,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -3753,11 +3753,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63618048"/>
-        <c:axId val="63620224"/>
+        <c:axId val="204760576"/>
+        <c:axId val="204762496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63618048"/>
+        <c:axId val="204760576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3786,7 +3786,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63620224"/>
+        <c:crossAx val="204762496"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3794,7 +3794,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63620224"/>
+        <c:axId val="204762496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3824,7 +3824,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63618048"/>
+        <c:crossAx val="204760576"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3840,7 +3840,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3853,10 +3853,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -4427,11 +4427,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63219584"/>
-        <c:axId val="63221760"/>
+        <c:axId val="203685248"/>
+        <c:axId val="204162560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63219584"/>
+        <c:axId val="203685248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4460,7 +4460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63221760"/>
+        <c:crossAx val="204162560"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4468,7 +4468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63221760"/>
+        <c:axId val="204162560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4498,7 +4498,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63219584"/>
+        <c:crossAx val="203685248"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4514,7 +4514,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4527,10 +4527,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -5101,11 +5101,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63743104"/>
-        <c:axId val="63745024"/>
+        <c:axId val="204224000"/>
+        <c:axId val="204225920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63743104"/>
+        <c:axId val="204224000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5134,7 +5134,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63745024"/>
+        <c:crossAx val="204225920"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5142,7 +5142,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63745024"/>
+        <c:axId val="204225920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5172,7 +5172,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63743104"/>
+        <c:crossAx val="204224000"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5188,7 +5188,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5201,10 +5201,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="110"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="10"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -5703,18 +5703,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$AT$3:$AT$9</c:f>
@@ -5787,11 +5775,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63909888"/>
-        <c:axId val="63912192"/>
+        <c:axId val="203984256"/>
+        <c:axId val="203990528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63909888"/>
+        <c:axId val="203984256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5820,7 +5808,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63912192"/>
+        <c:crossAx val="203990528"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5828,7 +5816,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63912192"/>
+        <c:axId val="203990528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5858,7 +5846,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63909888"/>
+        <c:crossAx val="203984256"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5872,14 +5860,9 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:prstDash val="sysDot"/>
-    </a:ln>
-  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5892,10 +5875,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="110"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="10"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -6390,11 +6373,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63957632"/>
-        <c:axId val="63836928"/>
+        <c:axId val="204048640"/>
+        <c:axId val="204059008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63957632"/>
+        <c:axId val="204048640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6423,7 +6406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63836928"/>
+        <c:crossAx val="204059008"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6431,7 +6414,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63836928"/>
+        <c:axId val="204059008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6461,7 +6444,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63957632"/>
+        <c:crossAx val="204048640"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6477,7 +6460,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6490,10 +6473,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -6836,11 +6819,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63881216"/>
-        <c:axId val="63883136"/>
+        <c:axId val="204121216"/>
+        <c:axId val="204123136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63881216"/>
+        <c:axId val="204121216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6869,7 +6852,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63883136"/>
+        <c:crossAx val="204123136"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6877,7 +6860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63883136"/>
+        <c:axId val="204123136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6907,7 +6890,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63881216"/>
+        <c:crossAx val="204121216"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6923,7 +6906,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6936,10 +6919,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -7130,11 +7113,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="63986688"/>
-        <c:axId val="63992960"/>
+        <c:axId val="204553600"/>
+        <c:axId val="204563968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63986688"/>
+        <c:axId val="204553600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7163,7 +7146,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63992960"/>
+        <c:crossAx val="204563968"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7171,7 +7154,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63992960"/>
+        <c:axId val="204563968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7201,7 +7184,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63986688"/>
+        <c:crossAx val="204553600"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7217,7 +7200,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7230,10 +7213,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -7728,11 +7711,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="64108032"/>
-        <c:axId val="64109952"/>
+        <c:axId val="204701696"/>
+        <c:axId val="204703616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64108032"/>
+        <c:axId val="204701696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7761,7 +7744,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64109952"/>
+        <c:crossAx val="204703616"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7769,7 +7752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64109952"/>
+        <c:axId val="204703616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7799,7 +7782,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64108032"/>
+        <c:crossAx val="204701696"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7815,7 +7798,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7828,10 +7811,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="118"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="18"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -8174,11 +8157,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="64145664"/>
-        <c:axId val="64156032"/>
+        <c:axId val="204302592"/>
+        <c:axId val="204308864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64145664"/>
+        <c:axId val="204302592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8207,7 +8190,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64156032"/>
+        <c:crossAx val="204308864"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8215,7 +8198,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64156032"/>
+        <c:axId val="204308864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8245,7 +8228,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64145664"/>
+        <c:crossAx val="204302592"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8261,7 +8244,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8588,7 +8571,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>74</xdr:col>
-      <xdr:colOff>800541</xdr:colOff>
+      <xdr:colOff>800540</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>46037</xdr:rowOff>
     </xdr:to>
@@ -9063,15 +9046,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CI232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BR54" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="CK110" sqref="CK110"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625"/>
     <col min="2" max="2" width="11.6640625"/>
-    <col min="3" max="3" width="26.33203125"/>
+    <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="23"/>
     <col min="5" max="5" width="23.5546875"/>
     <col min="6" max="6" width="26.33203125"/>
@@ -11237,7 +11220,7 @@
         <v>477.83500600000002</v>
       </c>
       <c r="CH9">
-        <f t="shared" si="27"/>
+        <f>SUM(AP68:AP77)/10000000</f>
         <v>1041.8468662</v>
       </c>
     </row>

</xml_diff>